<commit_message>
Remove CDN dependencies and fix bugs.
</commit_message>
<xml_diff>
--- a/scores.xlsx
+++ b/scores.xlsx
@@ -8,7 +8,6 @@
   </bookViews>
   <sheets>
     <sheet name="Men's Club Championship (Nett)" sheetId="1" r:id="rId1"/>
-    <sheet name="Men's Club Championship (Gross)" sheetId="2" r:id="rId2"/>
   </sheets>
   <calcPr calcId="140000" concurrentCalc="0"/>
   <extLst>
@@ -20,64 +19,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="28" uniqueCount="28">
-  <si>
-    <t>player</t>
-  </si>
-  <si>
-    <t>Test Player 1</t>
-  </si>
-  <si>
-    <t>Test Player 2</t>
-  </si>
-  <si>
-    <t>Test Player 3</t>
-  </si>
-  <si>
-    <t>Test Player 4</t>
-  </si>
-  <si>
-    <t>Test Player 5</t>
-  </si>
-  <si>
-    <t>Test Player 6</t>
-  </si>
-  <si>
-    <t>Test Player 7</t>
-  </si>
-  <si>
-    <t>Test Player 8</t>
-  </si>
-  <si>
-    <t>Test Player 9</t>
-  </si>
-  <si>
-    <t>Test Player 10</t>
-  </si>
-  <si>
-    <t>Test Player 11</t>
-  </si>
-  <si>
-    <t>Test Player 12</t>
-  </si>
-  <si>
-    <t>Test Player 13</t>
-  </si>
-  <si>
-    <t>Test Player 14</t>
-  </si>
-  <si>
-    <t>Test Player 15</t>
-  </si>
-  <si>
-    <t>Test Player 16</t>
-  </si>
-  <si>
-    <t>gross</t>
-  </si>
-  <si>
-    <t>Test Player 17</t>
-  </si>
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="14" uniqueCount="14">
   <si>
     <t>Player</t>
   </si>
@@ -104,16 +46,47 @@
   </si>
   <si>
     <t>R2</t>
+  </si>
+  <si>
+    <t>Total</t>
+  </si>
+  <si>
+    <t>Player 7</t>
+  </si>
+  <si>
+    <t>Player 8</t>
+  </si>
+  <si>
+    <t>Player 9</t>
+  </si>
+  <si>
+    <t>Player 10</t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <fonts count="1" x14ac:knownFonts="1">
+  <fonts count="3" x14ac:knownFonts="1">
     <font>
       <sz val="12"/>
       <color theme="1"/>
+      <name val="Calibri"/>
+      <family val="2"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <u/>
+      <sz val="12"/>
+      <color theme="10"/>
+      <name val="Calibri"/>
+      <family val="2"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <u/>
+      <sz val="12"/>
+      <color theme="11"/>
       <name val="Calibri"/>
       <family val="2"/>
       <scheme val="minor"/>
@@ -136,13 +109,41 @@
       <diagonal/>
     </border>
   </borders>
-  <cellStyleXfs count="1">
+  <cellStyleXfs count="15">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
   <cellXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
   </cellXfs>
-  <cellStyles count="1">
+  <cellStyles count="15">
+    <cellStyle name="Followed Hyperlink" xfId="2" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="4" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="6" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="8" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="10" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="12" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="14" builtinId="9" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="1" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="3" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="5" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="7" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="9" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="11" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="13" builtinId="8" hidden="1"/>
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
   </cellStyles>
   <dxfs count="0"/>
@@ -472,10 +473,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:C7"/>
+  <dimension ref="A1:D11"/>
   <sheetViews>
     <sheetView tabSelected="1" showRuler="0" workbookViewId="0">
-      <selection activeCell="C8" sqref="C8"/>
+      <selection activeCell="C2" sqref="C2:C11"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0"/>
@@ -483,20 +484,23 @@
     <col min="1" max="1" width="22.33203125" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:3">
+    <row r="1" spans="1:4">
       <c r="A1" t="s">
-        <v>19</v>
+        <v>0</v>
       </c>
       <c r="B1" t="s">
-        <v>20</v>
+        <v>1</v>
       </c>
       <c r="C1" t="s">
-        <v>27</v>
-      </c>
-    </row>
-    <row r="2" spans="1:3">
+        <v>8</v>
+      </c>
+      <c r="D1" t="s">
+        <v>9</v>
+      </c>
+    </row>
+    <row r="2" spans="1:4">
       <c r="A2" t="s">
-        <v>26</v>
+        <v>7</v>
       </c>
       <c r="B2">
         <v>72</v>
@@ -504,10 +508,14 @@
       <c r="C2">
         <v>73</v>
       </c>
-    </row>
-    <row r="3" spans="1:3">
+      <c r="D2">
+        <f>B2+C2</f>
+        <v>145</v>
+      </c>
+    </row>
+    <row r="3" spans="1:4">
       <c r="A3" t="s">
-        <v>21</v>
+        <v>11</v>
       </c>
       <c r="B3">
         <v>73</v>
@@ -515,49 +523,129 @@
       <c r="C3">
         <v>73</v>
       </c>
-    </row>
-    <row r="4" spans="1:3">
+      <c r="D3">
+        <f>B3+C3</f>
+        <v>146</v>
+      </c>
+    </row>
+    <row r="4" spans="1:4">
       <c r="A4" t="s">
-        <v>25</v>
+        <v>2</v>
       </c>
       <c r="B4">
+        <v>73</v>
+      </c>
+      <c r="C4">
+        <v>73</v>
+      </c>
+      <c r="D4">
+        <f t="shared" ref="D4:D11" si="0">B4+C4</f>
+        <v>146</v>
+      </c>
+    </row>
+    <row r="5" spans="1:4">
+      <c r="A5" t="s">
+        <v>6</v>
+      </c>
+      <c r="B5">
         <v>74</v>
       </c>
-      <c r="C4">
+      <c r="C5">
         <v>74</v>
       </c>
-    </row>
-    <row r="5" spans="1:3">
-      <c r="A5" t="s">
-        <v>22</v>
-      </c>
-      <c r="B5">
+      <c r="D5">
+        <f>B5+C5</f>
+        <v>148</v>
+      </c>
+    </row>
+    <row r="6" spans="1:4">
+      <c r="A6" t="s">
+        <v>12</v>
+      </c>
+      <c r="B6">
+        <v>79</v>
+      </c>
+      <c r="C6">
+        <v>70</v>
+      </c>
+      <c r="D6">
+        <f>B6+C6</f>
+        <v>149</v>
+      </c>
+    </row>
+    <row r="7" spans="1:4">
+      <c r="A7" t="s">
+        <v>10</v>
+      </c>
+      <c r="B7">
+        <v>74</v>
+      </c>
+      <c r="C7">
         <v>76</v>
       </c>
-      <c r="C5">
+      <c r="D7">
+        <f>B7+C7</f>
+        <v>150</v>
+      </c>
+    </row>
+    <row r="8" spans="1:4">
+      <c r="A8" t="s">
+        <v>3</v>
+      </c>
+      <c r="B8">
+        <v>76</v>
+      </c>
+      <c r="C8">
         <v>77</v>
       </c>
-    </row>
-    <row r="6" spans="1:3">
-      <c r="A6" t="s">
-        <v>23</v>
-      </c>
-      <c r="B6">
+      <c r="D8">
+        <f t="shared" si="0"/>
+        <v>153</v>
+      </c>
+    </row>
+    <row r="9" spans="1:4">
+      <c r="A9" t="s">
+        <v>4</v>
+      </c>
+      <c r="B9">
         <v>77</v>
       </c>
-      <c r="C6">
+      <c r="C9">
         <v>78</v>
       </c>
-    </row>
-    <row r="7" spans="1:3">
-      <c r="A7" t="s">
-        <v>24</v>
-      </c>
-      <c r="B7">
+      <c r="D9">
+        <f t="shared" si="0"/>
+        <v>155</v>
+      </c>
+    </row>
+    <row r="10" spans="1:4">
+      <c r="A10" t="s">
+        <v>13</v>
+      </c>
+      <c r="B10">
+        <v>80</v>
+      </c>
+      <c r="C10">
+        <v>82</v>
+      </c>
+      <c r="D10">
+        <f>B10+C10</f>
+        <v>162</v>
+      </c>
+    </row>
+    <row r="11" spans="1:4">
+      <c r="A11" t="s">
+        <v>5</v>
+      </c>
+      <c r="B11">
         <v>78</v>
       </c>
-      <c r="C7">
+      <c r="C11">
         <v>90</v>
+      </c>
+      <c r="D11">
+        <f t="shared" si="0"/>
+        <v>168</v>
       </c>
     </row>
   </sheetData>
@@ -565,188 +653,7 @@
     <sortCondition ref="B2"/>
   </sortState>
   <pageMargins left="0.75" right="0.75" top="1" bottom="1" header="0.5" footer="0.5"/>
-  <extLst>
-    <ext xmlns:mx="http://schemas.microsoft.com/office/mac/excel/2008/main" uri="{64002731-A6B0-56B0-2670-7721B7C09600}">
-      <mx:PLV Mode="0" OnePage="0" WScale="0"/>
-    </ext>
-  </extLst>
-</worksheet>
-</file>
-
-<file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:B18"/>
-  <sheetViews>
-    <sheetView showRuler="0" workbookViewId="0">
-      <selection activeCell="A5" sqref="A5:XFD5"/>
-    </sheetView>
-  </sheetViews>
-  <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0"/>
-  <cols>
-    <col min="1" max="1" width="22.33203125" customWidth="1"/>
-  </cols>
-  <sheetData>
-    <row r="1" spans="1:2">
-      <c r="A1" t="s">
-        <v>0</v>
-      </c>
-      <c r="B1" t="s">
-        <v>17</v>
-      </c>
-    </row>
-    <row r="2" spans="1:2">
-      <c r="A2" t="s">
-        <v>3</v>
-      </c>
-      <c r="B2">
-        <f t="shared" ref="B2:B17" ca="1" si="0">RANDBETWEEN(70, 85)</f>
-        <v>82</v>
-      </c>
-    </row>
-    <row r="3" spans="1:2">
-      <c r="A3" t="s">
-        <v>1</v>
-      </c>
-      <c r="B3">
-        <f ca="1">RANDBETWEEN(70, 85)</f>
-        <v>76</v>
-      </c>
-    </row>
-    <row r="4" spans="1:2">
-      <c r="A4" t="s">
-        <v>2</v>
-      </c>
-      <c r="B4">
-        <f t="shared" ca="1" si="0"/>
-        <v>73</v>
-      </c>
-    </row>
-    <row r="5" spans="1:2">
-      <c r="A5" t="s">
-        <v>4</v>
-      </c>
-      <c r="B5">
-        <f t="shared" ca="1" si="0"/>
-        <v>71</v>
-      </c>
-    </row>
-    <row r="6" spans="1:2">
-      <c r="A6" t="s">
-        <v>5</v>
-      </c>
-      <c r="B6">
-        <f t="shared" ca="1" si="0"/>
-        <v>72</v>
-      </c>
-    </row>
-    <row r="7" spans="1:2">
-      <c r="A7" t="s">
-        <v>6</v>
-      </c>
-      <c r="B7">
-        <f t="shared" ca="1" si="0"/>
-        <v>81</v>
-      </c>
-    </row>
-    <row r="8" spans="1:2">
-      <c r="A8" t="s">
-        <v>7</v>
-      </c>
-      <c r="B8">
-        <f t="shared" ca="1" si="0"/>
-        <v>81</v>
-      </c>
-    </row>
-    <row r="9" spans="1:2">
-      <c r="A9" t="s">
-        <v>8</v>
-      </c>
-      <c r="B9">
-        <f t="shared" ca="1" si="0"/>
-        <v>78</v>
-      </c>
-    </row>
-    <row r="10" spans="1:2">
-      <c r="A10" t="s">
-        <v>9</v>
-      </c>
-      <c r="B10">
-        <f t="shared" ca="1" si="0"/>
-        <v>76</v>
-      </c>
-    </row>
-    <row r="11" spans="1:2">
-      <c r="A11" t="s">
-        <v>10</v>
-      </c>
-      <c r="B11">
-        <v>93</v>
-      </c>
-    </row>
-    <row r="12" spans="1:2">
-      <c r="A12" t="s">
-        <v>11</v>
-      </c>
-      <c r="B12">
-        <f t="shared" ca="1" si="0"/>
-        <v>85</v>
-      </c>
-    </row>
-    <row r="13" spans="1:2">
-      <c r="A13" t="s">
-        <v>12</v>
-      </c>
-      <c r="B13">
-        <f t="shared" ca="1" si="0"/>
-        <v>75</v>
-      </c>
-    </row>
-    <row r="14" spans="1:2">
-      <c r="A14" t="s">
-        <v>13</v>
-      </c>
-      <c r="B14">
-        <f t="shared" ca="1" si="0"/>
-        <v>81</v>
-      </c>
-    </row>
-    <row r="15" spans="1:2">
-      <c r="A15" t="s">
-        <v>14</v>
-      </c>
-      <c r="B15">
-        <f t="shared" ca="1" si="0"/>
-        <v>70</v>
-      </c>
-    </row>
-    <row r="16" spans="1:2">
-      <c r="A16" t="s">
-        <v>15</v>
-      </c>
-      <c r="B16">
-        <f t="shared" ca="1" si="0"/>
-        <v>82</v>
-      </c>
-    </row>
-    <row r="17" spans="1:2">
-      <c r="A17" t="s">
-        <v>16</v>
-      </c>
-      <c r="B17">
-        <f t="shared" ca="1" si="0"/>
-        <v>84</v>
-      </c>
-    </row>
-    <row r="18" spans="1:2">
-      <c r="A18" t="s">
-        <v>18</v>
-      </c>
-      <c r="B18">
-        <v>69</v>
-      </c>
-    </row>
-  </sheetData>
-  <pageMargins left="0.75" right="0.75" top="1" bottom="1" header="0.5" footer="0.5"/>
+  <pageSetup paperSize="9" orientation="portrait" horizontalDpi="4294967292" verticalDpi="4294967292"/>
   <extLst>
     <ext xmlns:mx="http://schemas.microsoft.com/office/mac/excel/2008/main" uri="{64002731-A6B0-56B0-2670-7721B7C09600}">
       <mx:PLV Mode="0" OnePage="0" WScale="0"/>

</xml_diff>

<commit_message>
Use Go modules for dependencies and handle non returns correctly.
</commit_message>
<xml_diff>
--- a/scores.xlsx
+++ b/scores.xlsx
@@ -1,16 +1,28 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
-<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
-  <fileVersion appName="xl" lastEdited="5" lowestEdited="5" rupBuild="25007"/>
+<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="5" rupBuild="10609"/>
   <workbookPr showInkAnnotation="0" autoCompressPictures="0"/>
+  <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
+    <mc:Choice Requires="x15">
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/Chris/Projects/LiveLeaderboard/"/>
+    </mc:Choice>
+  </mc:AlternateContent>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{8852E67B-307B-9548-B814-7CFD158C092E}" xr6:coauthVersionLast="43" xr6:coauthVersionMax="43" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="23560" yWindow="4760" windowWidth="25600" windowHeight="19020" tabRatio="500"/>
+    <workbookView xWindow="23560" yWindow="4760" windowWidth="25600" windowHeight="19020" tabRatio="500" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Men's Club Championship (Nett)" sheetId="1" r:id="rId1"/>
   </sheets>
-  <calcPr calcId="140000" concurrentCalc="0"/>
+  <calcPr calcId="191029"/>
   <extLst>
+    <ext xmlns:xcalcf="http://schemas.microsoft.com/office/spreadsheetml/2018/calcfeatures" uri="{B58B0392-4F1F-4190-BB64-5DF3571DCE5F}">
+      <xcalcf:calcFeatures>
+        <xcalcf:feature name="microsoft.com:RD"/>
+        <xcalcf:feature name="microsoft.com:FV"/>
+      </xcalcf:calcFeatures>
+    </ext>
     <ext xmlns:mx="http://schemas.microsoft.com/office/mac/excel/2008/main" uri="{7523E5D3-25F3-A5E0-1632-64F254C22452}">
       <mx:ArchID Flags="2"/>
     </ext>
@@ -19,7 +31,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="14" uniqueCount="14">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="18" uniqueCount="16">
   <si>
     <t>Player</t>
   </si>
@@ -61,12 +73,18 @@
   </si>
   <si>
     <t>Player 10</t>
+  </si>
+  <si>
+    <t>Player 11</t>
+  </si>
+  <si>
+    <t>N/R</t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
-<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
   <fonts count="3" x14ac:knownFonts="1">
     <font>
       <sz val="12"/>
@@ -148,6 +166,14 @@
   </cellStyles>
   <dxfs count="0"/>
   <tableStyles count="0" defaultTableStyle="TableStyleMedium9" defaultPivotStyle="PivotStyleMedium4"/>
+  <extLst>
+    <ext xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" uri="{EB79DEF2-80B8-43e5-95BD-54CBDDF9020C}">
+      <x14:slicerStyles defaultSlicerStyle="SlicerStyleLight1"/>
+    </ext>
+    <ext xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" uri="{9260A510-F301-46a8-8635-F512D64BE5F5}">
+      <x15:timelineStyles defaultTimelineStyle="TimeSlicerStyleLight1"/>
+    </ext>
+  </extLst>
 </styleSheet>
 </file>
 
@@ -472,19 +498,19 @@
 </file>
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:D11"/>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
+  <dimension ref="A1:D12"/>
   <sheetViews>
     <sheetView tabSelected="1" showRuler="0" workbookViewId="0">
-      <selection activeCell="C2" sqref="C2:C11"/>
+      <selection activeCell="E12" sqref="E12"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0"/>
+  <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
   <cols>
     <col min="1" max="1" width="22.33203125" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:4">
+    <row r="1" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A1" t="s">
         <v>0</v>
       </c>
@@ -498,7 +524,7 @@
         <v>9</v>
       </c>
     </row>
-    <row r="2" spans="1:4">
+    <row r="2" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A2" t="s">
         <v>7</v>
       </c>
@@ -513,7 +539,7 @@
         <v>145</v>
       </c>
     </row>
-    <row r="3" spans="1:4">
+    <row r="3" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A3" t="s">
         <v>11</v>
       </c>
@@ -528,7 +554,7 @@
         <v>146</v>
       </c>
     </row>
-    <row r="4" spans="1:4">
+    <row r="4" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A4" t="s">
         <v>2</v>
       </c>
@@ -543,7 +569,7 @@
         <v>146</v>
       </c>
     </row>
-    <row r="5" spans="1:4">
+    <row r="5" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A5" t="s">
         <v>6</v>
       </c>
@@ -558,7 +584,7 @@
         <v>148</v>
       </c>
     </row>
-    <row r="6" spans="1:4">
+    <row r="6" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A6" t="s">
         <v>12</v>
       </c>
@@ -573,7 +599,7 @@
         <v>149</v>
       </c>
     </row>
-    <row r="7" spans="1:4">
+    <row r="7" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A7" t="s">
         <v>10</v>
       </c>
@@ -588,7 +614,7 @@
         <v>150</v>
       </c>
     </row>
-    <row r="8" spans="1:4">
+    <row r="8" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A8" t="s">
         <v>3</v>
       </c>
@@ -603,7 +629,7 @@
         <v>153</v>
       </c>
     </row>
-    <row r="9" spans="1:4">
+    <row r="9" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A9" t="s">
         <v>4</v>
       </c>
@@ -618,7 +644,7 @@
         <v>155</v>
       </c>
     </row>
-    <row r="10" spans="1:4">
+    <row r="10" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A10" t="s">
         <v>13</v>
       </c>
@@ -633,7 +659,7 @@
         <v>162</v>
       </c>
     </row>
-    <row r="11" spans="1:4">
+    <row r="11" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A11" t="s">
         <v>5</v>
       </c>
@@ -648,8 +674,22 @@
         <v>168</v>
       </c>
     </row>
+    <row r="12" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="A12" t="s">
+        <v>14</v>
+      </c>
+      <c r="B12" t="s">
+        <v>15</v>
+      </c>
+      <c r="C12" t="s">
+        <v>15</v>
+      </c>
+      <c r="D12" t="s">
+        <v>15</v>
+      </c>
+    </row>
   </sheetData>
-  <sortState ref="A2:B17">
+  <sortState xmlns:xlrd2="http://schemas.microsoft.com/office/spreadsheetml/2017/richdata2" ref="A2:B17">
     <sortCondition ref="B2"/>
   </sortState>
   <pageMargins left="0.75" right="0.75" top="1" bottom="1" header="0.5" footer="0.5"/>

</xml_diff>